<commit_message>
Penambahan dan Update API dan Model
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Master.TblPerson.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Master.TblPerson.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2514" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2534" uniqueCount="1204">
   <si>
     <t>Abd Samad</t>
   </si>
@@ -3565,6 +3565,69 @@
   </si>
   <si>
     <t>SYS_PID</t>
+  </si>
+  <si>
+    <t>Wisnu Andra Isdianto</t>
+  </si>
+  <si>
+    <t>khamim</t>
+  </si>
+  <si>
+    <t>Khamim</t>
+  </si>
+  <si>
+    <t>Slamet Riadi</t>
+  </si>
+  <si>
+    <t>Adythia Adikara</t>
+  </si>
+  <si>
+    <t>Agus Sopyan Hadi</t>
+  </si>
+  <si>
+    <t>Rafi Artman Siddiq</t>
+  </si>
+  <si>
+    <t>Azis Purwandana</t>
+  </si>
+  <si>
+    <t>Heryanto</t>
+  </si>
+  <si>
+    <t>Imran</t>
+  </si>
+  <si>
+    <t>Riza</t>
+  </si>
+  <si>
+    <t>wisnu.andra</t>
+  </si>
+  <si>
+    <t>riza</t>
+  </si>
+  <si>
+    <t>slametr</t>
+  </si>
+  <si>
+    <t>adythiaa</t>
+  </si>
+  <si>
+    <t>aguss</t>
+  </si>
+  <si>
+    <t>azisp</t>
+  </si>
+  <si>
+    <t>heryanto</t>
+  </si>
+  <si>
+    <t>imran</t>
+  </si>
+  <si>
+    <t>rafi.artman</t>
+  </si>
+  <si>
+    <t>Zaire Dite Biscaya</t>
   </si>
 </sst>
 </file>
@@ -3625,7 +3688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3633,6 +3696,7 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3937,15 +4001,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F502"/>
+  <dimension ref="A1:F512"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
+      <selection activeCell="B500" sqref="B500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="1"/>
@@ -10611,7 +10675,7 @@
         <v>488</v>
       </c>
       <c r="D445" s="1" t="str">
-        <f t="shared" ref="D445:D502" si="7">IF(EXACT(B445, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblPerson_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '", B445, "', null);"))</f>
+        <f t="shared" ref="D445:D507" si="7">IF(EXACT(B445, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblPerson_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '", B445, "', null);"))</f>
         <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Tjhang Linawati', null);</v>
       </c>
       <c r="F445" s="3">
@@ -11383,7 +11447,7 @@
         <v>25000000000495</v>
       </c>
     </row>
-    <row r="497" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B497" s="1" t="s">
         <v>262</v>
       </c>
@@ -11398,7 +11462,7 @@
         <v>25000000000496</v>
       </c>
     </row>
-    <row r="498" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B498" s="1" t="s">
         <v>1084</v>
       </c>
@@ -11413,22 +11477,22 @@
         <v>25000000000497</v>
       </c>
     </row>
-    <row r="499" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B499" s="1" t="s">
-        <v>512</v>
+        <v>1203</v>
       </c>
       <c r="C499" s="1" t="s">
         <v>513</v>
       </c>
       <c r="D499" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Zaire Dite', null);</v>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Zaire Dite Biscaya', null);</v>
       </c>
       <c r="F499" s="3">
         <v>25000000000498</v>
       </c>
     </row>
-    <row r="500" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B500" s="1" t="s">
         <v>264</v>
       </c>
@@ -11443,7 +11507,7 @@
         <v>25000000000499</v>
       </c>
     </row>
-    <row r="501" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B501" s="1" t="s">
         <v>1044</v>
       </c>
@@ -11458,7 +11522,7 @@
         <v>25000000000500</v>
       </c>
     </row>
-    <row r="502" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B502" s="1" t="s">
         <v>682</v>
       </c>
@@ -11471,6 +11535,159 @@
       </c>
       <c r="F502" s="3">
         <v>25000000000501</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A503" s="5">
+        <v>44491</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D503" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Adythia Adikara', null);</v>
+      </c>
+      <c r="F503" s="3">
+        <v>25000000000502</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B504" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D504" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Agus Sopyan Hadi', null);</v>
+      </c>
+      <c r="F504" s="3">
+        <v>25000000000503</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B505" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D505" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Azis Purwandana', null);</v>
+      </c>
+      <c r="F505" s="3">
+        <v>25000000000504</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B506" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D506" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Heryanto', null);</v>
+      </c>
+      <c r="F506" s="3">
+        <v>25000000000505</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B507" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D507" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Imran', null);</v>
+      </c>
+      <c r="F507" s="3">
+        <v>25000000000506</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B508" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D508" s="1" t="str">
+        <f t="shared" ref="D508:D512" si="8">IF(EXACT(B508, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblPerson_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, '", B508, "', null);"))</f>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Khamim', null);</v>
+      </c>
+      <c r="F508" s="3">
+        <v>25000000000507</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B509" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D509" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Rafi Artman Siddiq', null);</v>
+      </c>
+      <c r="F509" s="3">
+        <v>25000000000508</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B510" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D510" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Riza', null);</v>
+      </c>
+      <c r="F510" s="3">
+        <v>25000000000509</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B511" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D511" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Slamet Riadi', null);</v>
+      </c>
+      <c r="F511" s="3">
+        <v>25000000000510</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B512" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D512" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 'Wisnu Andra Isdianto', null);</v>
+      </c>
+      <c r="F512" s="3">
+        <v>25000000000511</v>
       </c>
     </row>
   </sheetData>
@@ -11483,7 +11700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B486"/>
   <sheetViews>
-    <sheetView topLeftCell="A390" workbookViewId="0">
+    <sheetView topLeftCell="A483" workbookViewId="0">
       <selection activeCell="B450" sqref="B450"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update List User Samba (Penambahan adhe.kurniawan, eka.kurniawan, eka.purwanti, fikri, marungkil)
Penambahan Record untuk Excel SQL Generator
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Master.TblPerson.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Master.TblPerson.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="1373">
   <si>
     <t>Abd Samad</t>
   </si>
@@ -4101,6 +4101,42 @@
   </si>
   <si>
     <t>Sys_PID</t>
+  </si>
+  <si>
+    <t>Firmansyah Awaludin</t>
+  </si>
+  <si>
+    <t>Syafri Johansah</t>
+  </si>
+  <si>
+    <t>Iman Faisal Abdurahman</t>
+  </si>
+  <si>
+    <t>Budi Sandika</t>
+  </si>
+  <si>
+    <t>Fachri Azhar</t>
+  </si>
+  <si>
+    <t>Muhammad Irfan Alfikri</t>
+  </si>
+  <si>
+    <t>firmansyah.awaludin</t>
+  </si>
+  <si>
+    <t>syafri.johansah</t>
+  </si>
+  <si>
+    <t>budi.sandika</t>
+  </si>
+  <si>
+    <t>fachri.azhar</t>
+  </si>
+  <si>
+    <t>Iman.faisal</t>
+  </si>
+  <si>
+    <t>muhammad.irfan</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4497,35 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4795,14 +4859,14 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I589"/>
+  <dimension ref="A1:I595"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C434" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C583" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C12" sqref="C12"/>
       <selection pane="topRight" activeCell="C12" sqref="C12"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
-      <selection pane="bottomRight" activeCell="F442" sqref="F442"/>
+      <selection pane="bottomRight" activeCell="A590" sqref="A590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16880,7 +16944,7 @@
         <v>Musdalipa</v>
       </c>
     </row>
-    <row r="577" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B577" s="10" t="s">
         <v>1346</v>
       </c>
@@ -16901,7 +16965,7 @@
         <v>Nico Melky</v>
       </c>
     </row>
-    <row r="578" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B578" s="10" t="s">
         <v>1338</v>
       </c>
@@ -16922,7 +16986,7 @@
         <v>Rahmata Novanisa</v>
       </c>
     </row>
-    <row r="579" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B579" s="10" t="s">
         <v>1352</v>
       </c>
@@ -16943,7 +17007,7 @@
         <v>Satrio Dhiaputra</v>
       </c>
     </row>
-    <row r="580" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B580" s="10" t="s">
         <v>1308</v>
       </c>
@@ -16964,7 +17028,7 @@
         <v>Sudirman</v>
       </c>
     </row>
-    <row r="581" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B581" s="10" t="s">
         <v>1340</v>
       </c>
@@ -16973,11 +17037,11 @@
       </c>
       <c r="D581" s="21"/>
       <c r="F581" s="23">
-        <f t="shared" ref="F581:F588" si="29" xml:space="preserve"> F580 + IF(EXACT(G581, ""), 0, 1)</f>
+        <f t="shared" ref="F581:F594" si="29" xml:space="preserve"> F580 + IF(EXACT(G581, ""), 0, 1)</f>
         <v>25000000000578</v>
       </c>
       <c r="G581" s="24" t="str">
-        <f t="shared" ref="G581:G588" si="30">IF(EXACT(B581, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblPerson_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B581, "'::varchar, null::bigint);"))</f>
+        <f t="shared" ref="G581:G594" si="30">IF(EXACT(B581, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblPerson_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B581, "'::varchar, null::bigint);"))</f>
         <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Suparji'::varchar, null::bigint);</v>
       </c>
       <c r="I581" s="1" t="str">
@@ -16985,7 +17049,7 @@
         <v>Suparji</v>
       </c>
     </row>
-    <row r="582" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B582" s="10" t="s">
         <v>1342</v>
       </c>
@@ -17006,7 +17070,7 @@
         <v>Taufik Iskandar</v>
       </c>
     </row>
-    <row r="583" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B583" s="10" t="s">
         <v>1329</v>
       </c>
@@ -17027,7 +17091,7 @@
         <v>Tegar Hersaputra</v>
       </c>
     </row>
-    <row r="584" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B584" s="10" t="s">
         <v>1301</v>
       </c>
@@ -17048,7 +17112,7 @@
         <v>Togar Sihombing</v>
       </c>
     </row>
-    <row r="585" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B585" s="10" t="s">
         <v>1348</v>
       </c>
@@ -17069,7 +17133,7 @@
         <v>Wisnu Trenggono</v>
       </c>
     </row>
-    <row r="586" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B586" s="10" t="s">
         <v>1339</v>
       </c>
@@ -17090,7 +17154,7 @@
         <v>Yogo</v>
       </c>
     </row>
-    <row r="587" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B587" s="10" t="s">
         <v>1345</v>
       </c>
@@ -17111,14 +17175,14 @@
         <v>Yustiana Firda</v>
       </c>
     </row>
-    <row r="588" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B588" s="10" t="s">
+    <row r="588" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B588" s="11" t="s">
         <v>1299</v>
       </c>
-      <c r="C588" s="10" t="s">
+      <c r="C588" s="11" t="s">
         <v>1298</v>
       </c>
-      <c r="D588" s="21"/>
+      <c r="D588" s="22"/>
       <c r="F588" s="23">
         <f t="shared" si="29"/>
         <v>25000000000585</v>
@@ -17132,22 +17196,127 @@
         <v>Zainal Abidin</v>
       </c>
     </row>
-    <row r="589" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B589" s="11" t="str">
-        <f>IF(EXACT(MAIN!$F589, ""), "", MAIN!$F589)</f>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A589" s="4">
+        <v>45721</v>
+      </c>
+      <c r="B589" s="10" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C589" s="10" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D589" s="21"/>
+      <c r="F589" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000586</v>
+      </c>
+      <c r="G589" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Budi Sandika'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="590" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B590" s="10" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C590" s="10" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D590" s="21"/>
+      <c r="F590" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000587</v>
+      </c>
+      <c r="G590" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Fachri Azhar'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B591" s="10" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C591" s="10" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D591" s="21"/>
+      <c r="F591" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000588</v>
+      </c>
+      <c r="G591" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Firmansyah Awaludin'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="592" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B592" s="10" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C592" s="10" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D592" s="21"/>
+      <c r="F592" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000589</v>
+      </c>
+      <c r="G592" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Iman Faisal Abdurahman'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="593" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B593" s="10" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C593" s="10" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D593" s="21"/>
+      <c r="F593" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000590</v>
+      </c>
+      <c r="G593" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Muhammad Irfan Alfikri'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="594" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B594" s="10" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C594" s="10" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D594" s="21"/>
+      <c r="F594" s="23">
+        <f t="shared" si="29"/>
+        <v>25000000000591</v>
+      </c>
+      <c r="G594" s="24" t="str">
+        <f t="shared" si="30"/>
+        <v>PERFORM "SchData-OLTP-Master"."Func_TblPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'Syafri Johansah'::varchar, null::bigint);</v>
+      </c>
+    </row>
+    <row r="595" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B595" s="11" t="str">
+        <f>IF(EXACT(MAIN!$F595, ""), "", MAIN!$F595)</f>
         <v/>
       </c>
-      <c r="C589" s="11"/>
-      <c r="D589" s="22"/>
-      <c r="F589" s="25"/>
-      <c r="G589" s="11"/>
+      <c r="C595" s="11"/>
+      <c r="D595" s="22"/>
+      <c r="F595" s="25"/>
+      <c r="G595" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="B558:C586">
-    <sortCondition ref="B558:B586"/>
+  <sortState ref="B589:D594">
+    <sortCondition ref="B589"/>
   </sortState>
-  <conditionalFormatting sqref="F4:F588">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="F4:F594">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>EXACT(F3, F4)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17166,11 +17335,11 @@
   </sheetPr>
   <dimension ref="B1:C620"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C584" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="I598" sqref="I598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23045,70 +23214,105 @@
       </c>
     </row>
     <row r="589" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B589" s="30" t="str">
+      <c r="B589" s="29">
         <f>IF(EXACT(MAIN!$F589, ""), "", MAIN!$F589)</f>
-        <v/>
-      </c>
-      <c r="C589" s="33" t="str">
+        <v>25000000000586</v>
+      </c>
+      <c r="C589" s="32" t="str">
+        <f>IF(EXACT(MAIN!B589, ""), "", MAIN!B589)</f>
+        <v>Budi Sandika</v>
+      </c>
+    </row>
+    <row r="590" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B590" s="29">
+        <f>IF(EXACT(MAIN!$F590, ""), "", MAIN!$F590)</f>
+        <v>25000000000587</v>
+      </c>
+      <c r="C590" s="32" t="str">
         <f>IF(EXACT(MAIN!B590, ""), "", MAIN!B590)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="590" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B590" s="2"/>
+        <v>Fachri Azhar</v>
+      </c>
     </row>
     <row r="591" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B591" s="2"/>
+      <c r="B591" s="29">
+        <f>IF(EXACT(MAIN!$F591, ""), "", MAIN!$F591)</f>
+        <v>25000000000588</v>
+      </c>
+      <c r="C591" s="32" t="str">
+        <f>IF(EXACT(MAIN!B591, ""), "", MAIN!B591)</f>
+        <v>Firmansyah Awaludin</v>
+      </c>
     </row>
     <row r="592" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B592" s="2"/>
-    </row>
-    <row r="593" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B593" s="2"/>
-    </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B594" s="2"/>
-    </row>
-    <row r="595" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B592" s="29">
+        <f>IF(EXACT(MAIN!$F592, ""), "", MAIN!$F592)</f>
+        <v>25000000000589</v>
+      </c>
+      <c r="C592" s="32" t="str">
+        <f>IF(EXACT(MAIN!B592, ""), "", MAIN!B592)</f>
+        <v>Iman Faisal Abdurahman</v>
+      </c>
+    </row>
+    <row r="593" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B593" s="29">
+        <f>IF(EXACT(MAIN!$F593, ""), "", MAIN!$F593)</f>
+        <v>25000000000590</v>
+      </c>
+      <c r="C593" s="32" t="str">
+        <f>IF(EXACT(MAIN!B593, ""), "", MAIN!B593)</f>
+        <v>Muhammad Irfan Alfikri</v>
+      </c>
+    </row>
+    <row r="594" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B594" s="30">
+        <f>IF(EXACT(MAIN!$F594, ""), "", MAIN!$F594)</f>
+        <v>25000000000591</v>
+      </c>
+      <c r="C594" s="33" t="str">
+        <f>IF(EXACT(MAIN!B594, ""), "", MAIN!B594)</f>
+        <v>Syafri Johansah</v>
+      </c>
+    </row>
+    <row r="595" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B595" s="2"/>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="596" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B596" s="2"/>
     </row>
-    <row r="597" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="597" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B597" s="2"/>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="598" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B598" s="2"/>
     </row>
-    <row r="599" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="599" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B599" s="2"/>
     </row>
-    <row r="600" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="600" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B600" s="2"/>
     </row>
-    <row r="601" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="601" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B601" s="2"/>
     </row>
-    <row r="602" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="602" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B602" s="2"/>
     </row>
-    <row r="603" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="603" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B603" s="2"/>
     </row>
-    <row r="604" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="604" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B604" s="2"/>
     </row>
-    <row r="605" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="605" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B605" s="2"/>
     </row>
-    <row r="606" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="606" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B606" s="2"/>
     </row>
-    <row r="607" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="607" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B607" s="2"/>
     </row>
-    <row r="608" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="608" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B608" s="2"/>
     </row>
     <row r="609" spans="2:2" x14ac:dyDescent="0.2">
@@ -23156,7 +23360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B588"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A298" workbookViewId="0">
       <selection activeCell="H557" sqref="H557"/>
     </sheetView>
   </sheetViews>

</xml_diff>